<commit_message>
Final Notebook | 1st Part
</commit_message>
<xml_diff>
--- a/EDA_Outputs/Tables/Total_Number_Food_Types_Purchased.xlsx
+++ b/EDA_Outputs/Tables/Total_Number_Food_Types_Purchased.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>%</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>%_cumulative</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -460,6 +465,9 @@
       <c r="C2" t="n">
         <v>36.51</v>
       </c>
+      <c r="D2" t="n">
+        <v>36.51</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -471,6 +479,9 @@
       <c r="C3" t="n">
         <v>30.89</v>
       </c>
+      <c r="D3" t="n">
+        <v>67.40000000000001</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -482,6 +493,9 @@
       <c r="C4" t="n">
         <v>16.31</v>
       </c>
+      <c r="D4" t="n">
+        <v>83.71000000000001</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -493,6 +507,9 @@
       <c r="C5" t="n">
         <v>8.08</v>
       </c>
+      <c r="D5" t="n">
+        <v>91.79000000000001</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -504,6 +521,9 @@
       <c r="C6" t="n">
         <v>3.99</v>
       </c>
+      <c r="D6" t="n">
+        <v>95.78</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -515,6 +535,9 @@
       <c r="C7" t="n">
         <v>2.13</v>
       </c>
+      <c r="D7" t="n">
+        <v>97.91</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -526,6 +549,9 @@
       <c r="C8" t="n">
         <v>1.13</v>
       </c>
+      <c r="D8" t="n">
+        <v>99.03999999999999</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -537,6 +563,9 @@
       <c r="C9" t="n">
         <v>0.5600000000000001</v>
       </c>
+      <c r="D9" t="n">
+        <v>99.59999999999999</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -548,6 +577,9 @@
       <c r="C10" t="n">
         <v>0.21</v>
       </c>
+      <c r="D10" t="n">
+        <v>99.80999999999999</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -559,6 +591,9 @@
       <c r="C11" t="n">
         <v>0.11</v>
       </c>
+      <c r="D11" t="n">
+        <v>99.91999999999999</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -570,6 +605,9 @@
       <c r="C12" t="n">
         <v>0.06</v>
       </c>
+      <c r="D12" t="n">
+        <v>99.97999999999999</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -581,6 +619,9 @@
       <c r="C13" t="n">
         <v>0.01</v>
       </c>
+      <c r="D13" t="n">
+        <v>99.98999999999999</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -591,6 +632,9 @@
       </c>
       <c r="C14" t="n">
         <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>99.98999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>